<commit_message>
Added new data and dash tab
</commit_message>
<xml_diff>
--- a/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
+++ b/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Parking Lot\Web Projects\jc-farms\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CD5668A3-E2FE-4A7D-80AC-9FA456A5E4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD297C-857E-4F37-92FD-D787E5EF229E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="4" activeTab="5" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="20" activeTab="22" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
   </bookViews>
   <sheets>
     <sheet name="20250131 to 20250213" sheetId="15" r:id="rId1"/>
@@ -30,19 +30,21 @@
     <sheet name="Jospeh_PR_13M - 23M" sheetId="27" r:id="rId15"/>
     <sheet name="Joseph_PR_20M - 27M" sheetId="29" r:id="rId16"/>
     <sheet name="Nico_PR_16M to Sale" sheetId="28" r:id="rId17"/>
-    <sheet name="Template" sheetId="12" r:id="rId18"/>
-    <sheet name="&lt;&lt;&lt; Budget Forecasts" sheetId="16" r:id="rId19"/>
-    <sheet name="Detailed Financials &gt;&gt;" sheetId="17" r:id="rId20"/>
-    <sheet name="Model" sheetId="1" r:id="rId21"/>
-    <sheet name="P + L  Income Statement" sheetId="7" r:id="rId22"/>
-    <sheet name="Balance Sheet" sheetId="6" r:id="rId23"/>
-    <sheet name="Cash Flow Statement" sheetId="8" r:id="rId24"/>
-    <sheet name="Chicken House 2 - 300" sheetId="11" r:id="rId25"/>
-    <sheet name="Chicken House - 500" sheetId="2" r:id="rId26"/>
-    <sheet name="Guard House" sheetId="3" r:id="rId27"/>
-    <sheet name="Finishings" sheetId="4" r:id="rId28"/>
-    <sheet name="Floor and Stone Work" sheetId="5" r:id="rId29"/>
-    <sheet name="Sheet2" sheetId="18" r:id="rId30"/>
+    <sheet name="Nico_PR_25Mar to 8Apr" sheetId="31" r:id="rId18"/>
+    <sheet name="Template" sheetId="12" r:id="rId19"/>
+    <sheet name="&lt;&lt;&lt; Budget Forecasts" sheetId="16" r:id="rId20"/>
+    <sheet name="Detailed Financials &gt;&gt;" sheetId="17" r:id="rId21"/>
+    <sheet name="Model" sheetId="1" r:id="rId22"/>
+    <sheet name="PnL" sheetId="32" r:id="rId23"/>
+    <sheet name="P + L  Income Statement" sheetId="7" r:id="rId24"/>
+    <sheet name="Balance Sheet" sheetId="6" r:id="rId25"/>
+    <sheet name="Cash Flow Statement" sheetId="8" r:id="rId26"/>
+    <sheet name="Chicken House 2 - 300" sheetId="11" r:id="rId27"/>
+    <sheet name="Chicken House - 500" sheetId="2" r:id="rId28"/>
+    <sheet name="Guard House" sheetId="3" r:id="rId29"/>
+    <sheet name="Finishings" sheetId="4" r:id="rId30"/>
+    <sheet name="Floor and Stone Work" sheetId="5" r:id="rId31"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId32"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20250128 to 20250302'!$A$1:$AA$100</definedName>
@@ -51,7 +53,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId31"/>
+    <pivotCache cacheId="0" r:id="rId33"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -207,7 +209,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7597" uniqueCount="1377">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7661" uniqueCount="1383">
   <si>
     <t>A. Capital Expenditure (Capex)</t>
   </si>
@@ -4338,6 +4340,24 @@
   </si>
   <si>
     <t>Price went up to 1500</t>
+  </si>
+  <si>
+    <t>For Charcoal</t>
+  </si>
+  <si>
+    <t>For Wood Shavings</t>
+  </si>
+  <si>
+    <t>For Feeds and Vaccination</t>
+  </si>
+  <si>
+    <t>Full sacks</t>
+  </si>
+  <si>
+    <t>Sales Revenue</t>
+  </si>
+  <si>
+    <t>Operating Expenses (OPEX)</t>
   </si>
 </sst>
 </file>
@@ -16040,8 +16060,8 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView showGridLines="0" topLeftCell="B8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16802,7 +16822,7 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C27" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="C28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
@@ -17481,6 +17501,757 @@
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ED07ED4-8072-4C59-B21A-877F5BB85498}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O42"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A22" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+      <selection activeCell="N40" sqref="N40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="73" t="s">
+        <v>691</v>
+      </c>
+      <c r="B1" s="73"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E3" s="137" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="139"/>
+      <c r="N3" s="59"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="74" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="105">
+        <v>4</v>
+      </c>
+      <c r="F4" s="105">
+        <v>5</v>
+      </c>
+      <c r="G4" s="105">
+        <v>6</v>
+      </c>
+      <c r="H4" s="105">
+        <v>7</v>
+      </c>
+      <c r="I4" s="105">
+        <v>8</v>
+      </c>
+      <c r="J4" s="105">
+        <v>9</v>
+      </c>
+      <c r="K4" s="105">
+        <v>10</v>
+      </c>
+      <c r="L4" s="105">
+        <v>11</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="74" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="61" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="97"/>
+    </row>
+    <row r="7" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="97"/>
+    </row>
+    <row r="8" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="97"/>
+    </row>
+    <row r="9" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="97"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="61" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="N10" s="56"/>
+    </row>
+    <row r="11" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="96" t="s">
+        <v>700</v>
+      </c>
+      <c r="C11" s="97">
+        <v>120</v>
+      </c>
+      <c r="D11" s="98">
+        <v>1500</v>
+      </c>
+      <c r="E11" s="98"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98">
+        <f>C11*D11</f>
+        <v>180000</v>
+      </c>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="98">
+        <f>I11</f>
+        <v>180000</v>
+      </c>
+      <c r="O11" s="97"/>
+    </row>
+    <row r="12" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="96" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C12" s="97">
+        <v>50</v>
+      </c>
+      <c r="D12" s="98">
+        <v>4300</v>
+      </c>
+      <c r="E12" s="98"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98">
+        <f>C12*D12</f>
+        <v>215000</v>
+      </c>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="97"/>
+      <c r="N12" s="98">
+        <f>I12</f>
+        <v>215000</v>
+      </c>
+      <c r="O12" s="97"/>
+    </row>
+    <row r="13" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="96"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="97"/>
+    </row>
+    <row r="14" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="97"/>
+    </row>
+    <row r="15" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="96"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="97"/>
+    </row>
+    <row r="16" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="97"/>
+    </row>
+    <row r="17" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="97"/>
+    </row>
+    <row r="18" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="97"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="97"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="96" t="s">
+        <v>1379</v>
+      </c>
+      <c r="C20" s="97">
+        <v>1</v>
+      </c>
+      <c r="D20" s="98">
+        <v>10000</v>
+      </c>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="98">
+        <f>C20*D20</f>
+        <v>10000</v>
+      </c>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+      <c r="N20" s="98">
+        <f>I20</f>
+        <v>10000</v>
+      </c>
+      <c r="O20" s="97"/>
+    </row>
+    <row r="21" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="98"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="97"/>
+    </row>
+    <row r="22" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="96" t="s">
+        <v>1378</v>
+      </c>
+      <c r="C22" s="97">
+        <v>1</v>
+      </c>
+      <c r="D22" s="98">
+        <v>10000</v>
+      </c>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97"/>
+      <c r="I22" s="98">
+        <f>C22*D22</f>
+        <v>10000</v>
+      </c>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98">
+        <f>I22</f>
+        <v>10000</v>
+      </c>
+      <c r="O22" s="97"/>
+    </row>
+    <row r="23" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="96" t="s">
+        <v>1377</v>
+      </c>
+      <c r="C23" s="97">
+        <v>1</v>
+      </c>
+      <c r="D23" s="98">
+        <v>2000</v>
+      </c>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="97"/>
+      <c r="H23" s="97"/>
+      <c r="I23" s="98">
+        <f>C23*D23</f>
+        <v>2000</v>
+      </c>
+      <c r="J23" s="97"/>
+      <c r="K23" s="97"/>
+      <c r="L23" s="97"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="98">
+        <f>I23</f>
+        <v>2000</v>
+      </c>
+      <c r="O23" s="97"/>
+    </row>
+    <row r="24" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="96"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="99"/>
+      <c r="J24" s="99"/>
+      <c r="K24" s="99"/>
+      <c r="L24" s="99"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="97"/>
+    </row>
+    <row r="25" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B25" s="96"/>
+      <c r="C25" s="97"/>
+      <c r="D25" s="98"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="98"/>
+      <c r="G25" s="97"/>
+      <c r="H25" s="97"/>
+      <c r="I25" s="97"/>
+      <c r="J25" s="97"/>
+      <c r="K25" s="97"/>
+      <c r="L25" s="97"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="98"/>
+      <c r="O25" s="97"/>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B26" s="71" t="s">
+        <v>368</v>
+      </c>
+      <c r="D26" s="56"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="56"/>
+      <c r="N26" s="56"/>
+    </row>
+    <row r="27" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="96" t="s">
+        <v>1125</v>
+      </c>
+      <c r="C27" s="97">
+        <v>500</v>
+      </c>
+      <c r="D27" s="98">
+        <v>24</v>
+      </c>
+      <c r="E27" s="97"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="98">
+        <f>C27*D27</f>
+        <v>12000</v>
+      </c>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="98">
+        <f>I27</f>
+        <v>12000</v>
+      </c>
+      <c r="O27" s="97"/>
+    </row>
+    <row r="28" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="96"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="97"/>
+    </row>
+    <row r="29" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="97"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="97"/>
+      <c r="K29" s="97"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="97"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="97"/>
+    </row>
+    <row r="30" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="96"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="97"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="97"/>
+      <c r="H30" s="97"/>
+      <c r="I30" s="97"/>
+      <c r="J30" s="97"/>
+      <c r="K30" s="97"/>
+      <c r="L30" s="97"/>
+      <c r="M30" s="97"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="97"/>
+    </row>
+    <row r="31" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="96"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="99"/>
+      <c r="L31" s="99"/>
+      <c r="M31" s="97"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="97"/>
+    </row>
+    <row r="32" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B32" s="96"/>
+      <c r="C32" s="97"/>
+      <c r="D32" s="98"/>
+      <c r="E32" s="98"/>
+      <c r="F32" s="98"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="97"/>
+      <c r="K32" s="97"/>
+      <c r="L32" s="97"/>
+      <c r="M32" s="97"/>
+      <c r="N32" s="100"/>
+      <c r="O32" s="97"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B33" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="56"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="56"/>
+      <c r="N33" s="56"/>
+    </row>
+    <row r="34" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="96" t="s">
+        <v>1380</v>
+      </c>
+      <c r="C34" s="97">
+        <v>10</v>
+      </c>
+      <c r="D34" s="98">
+        <v>5000</v>
+      </c>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="98">
+        <f>C34*D34</f>
+        <v>50000</v>
+      </c>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="98">
+        <f>I34</f>
+        <v>50000</v>
+      </c>
+      <c r="O34" s="97"/>
+    </row>
+    <row r="35" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="96"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="97"/>
+      <c r="M35" s="97"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="97"/>
+    </row>
+    <row r="36" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B36" s="96"/>
+      <c r="C36" s="97"/>
+      <c r="D36" s="98"/>
+      <c r="E36" s="98"/>
+      <c r="F36" s="98"/>
+      <c r="G36" s="97"/>
+      <c r="H36" s="97"/>
+      <c r="I36" s="97"/>
+      <c r="J36" s="97"/>
+      <c r="K36" s="97"/>
+      <c r="L36" s="97"/>
+      <c r="M36" s="97"/>
+      <c r="N36" s="98"/>
+      <c r="O36" s="97"/>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B37" s="61" t="s">
+        <v>696</v>
+      </c>
+      <c r="N37" s="56"/>
+    </row>
+    <row r="38" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="96" t="s">
+        <v>559</v>
+      </c>
+      <c r="C38" s="97">
+        <v>1</v>
+      </c>
+      <c r="D38" s="97">
+        <v>75000</v>
+      </c>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="97"/>
+      <c r="H38" s="97"/>
+      <c r="I38" s="98">
+        <f>C38*D38</f>
+        <v>75000</v>
+      </c>
+      <c r="J38" s="97"/>
+      <c r="K38" s="97"/>
+      <c r="L38" s="97"/>
+      <c r="M38" s="97"/>
+      <c r="N38" s="98">
+        <f>I38</f>
+        <v>75000</v>
+      </c>
+      <c r="O38" s="97"/>
+    </row>
+    <row r="39" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="96" t="s">
+        <v>331</v>
+      </c>
+      <c r="C39" s="97">
+        <v>1</v>
+      </c>
+      <c r="D39" s="97">
+        <v>18000</v>
+      </c>
+      <c r="E39" s="97"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="98">
+        <f>C39*D39</f>
+        <v>18000</v>
+      </c>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="98">
+        <f>I39</f>
+        <v>18000</v>
+      </c>
+      <c r="O39" s="97"/>
+    </row>
+    <row r="40" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B40" s="97"/>
+      <c r="C40" s="97"/>
+      <c r="D40" s="97"/>
+      <c r="E40" s="97"/>
+      <c r="F40" s="97"/>
+      <c r="G40" s="97"/>
+      <c r="H40" s="97"/>
+      <c r="I40" s="97"/>
+      <c r="J40" s="97"/>
+      <c r="K40" s="97"/>
+      <c r="L40" s="97"/>
+      <c r="M40" s="97"/>
+      <c r="N40" s="98"/>
+      <c r="O40" s="97"/>
+    </row>
+    <row r="41" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B41" s="72"/>
+      <c r="C41" s="72"/>
+      <c r="D41" s="72"/>
+      <c r="E41" s="72"/>
+      <c r="F41" s="72"/>
+      <c r="G41" s="72"/>
+      <c r="H41" s="72"/>
+      <c r="I41" s="72"/>
+      <c r="J41" s="72"/>
+      <c r="K41" s="72"/>
+      <c r="L41" s="72"/>
+      <c r="M41" s="101" t="s">
+        <v>234</v>
+      </c>
+      <c r="N41" s="102">
+        <f>SUM(N5:N39)</f>
+        <v>572000</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="N42" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD012E-1301-4CDB-B54B-ED7FEAC48C53}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -18104,23 +18875,6 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B905C8F-AA7B-4366-ACBD-214566A869AE}">
-  <sheetPr>
-    <tabColor rgb="FF92D050"/>
-  </sheetPr>
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -21164,6 +21918,23 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B905C8F-AA7B-4366-ACBD-214566A869AE}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E000CEC5-651A-41CF-9370-A65672278D0D}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -21180,7 +21951,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A94399-3FA4-4BC1-8ACB-AC4F9CB00833}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -30594,16 +31365,16 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D568-367A-4BE4-A886-CC86E2F5DEA9}">
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B979F449-628E-4A37-A375-770828AACAA5}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -30724,21 +31495,21 @@
         <v>282</v>
       </c>
       <c r="D5" s="83">
-        <f>D6+D7</f>
+        <f>D6</f>
         <v>3266000</v>
       </c>
       <c r="E5" s="83">
-        <f>E6+E7</f>
+        <f t="shared" ref="E5:F5" si="0">E6</f>
         <v>3980500</v>
       </c>
       <c r="F5" s="83">
-        <f>F6+F7</f>
+        <f t="shared" si="0"/>
         <v>2870000</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
-        <v>245</v>
+        <v>1381</v>
       </c>
       <c r="C6" t="s">
         <v>246</v>
@@ -30756,405 +31527,263 @@
         <v>2870000</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B7" t="s">
-        <v>247</v>
-      </c>
-      <c r="C7" t="s">
-        <v>248</v>
-      </c>
-      <c r="D7">
-        <v>0</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B8" s="60" t="s">
+    <row r="7" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B7" s="60" t="s">
         <v>249</v>
       </c>
-      <c r="C8" s="61" t="s">
+      <c r="C7" s="61" t="s">
         <v>283</v>
       </c>
-      <c r="D8" s="64">
-        <f>SUM(D9:D12)</f>
+      <c r="D7" s="64">
+        <f>SUM(D8:D11)</f>
         <v>2532000</v>
       </c>
-      <c r="E8" s="64">
-        <f>SUM(E9:E12)</f>
+      <c r="E7" s="64">
+        <f>SUM(E8:E11)</f>
         <v>3149000</v>
       </c>
-      <c r="F8" s="64">
-        <f>SUM(F9:F12)</f>
+      <c r="F7" s="64">
+        <f>SUM(F8:F11)</f>
         <v>2050000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
+        <v>284</v>
+      </c>
+      <c r="D8" s="79">
+        <f>Model!I94</f>
+        <v>1850000</v>
+      </c>
+      <c r="E8" s="79">
+        <f>Model!J94</f>
+        <v>2110000</v>
+      </c>
+      <c r="F8" s="79">
+        <f>Model!K94</f>
+        <v>1393000</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="C9" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="D9" s="79">
-        <f>Model!I94</f>
-        <v>1850000</v>
+        <f>Model!I74</f>
+        <v>72000</v>
       </c>
       <c r="E9" s="79">
-        <f>Model!J94</f>
-        <v>2110000</v>
+        <f>Model!J74</f>
+        <v>59000</v>
       </c>
       <c r="F9" s="79">
-        <f>Model!K94</f>
-        <v>1393000</v>
+        <f>Model!K74</f>
+        <v>77000</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="C10" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="D10" s="79">
-        <f>Model!I74</f>
-        <v>72000</v>
+        <f>Model!I62</f>
+        <v>600000</v>
       </c>
       <c r="E10" s="79">
-        <f>Model!J74</f>
-        <v>59000</v>
+        <f>Model!J62</f>
+        <v>930000</v>
       </c>
       <c r="F10" s="79">
-        <f>Model!K74</f>
-        <v>77000</v>
+        <f>Model!K62</f>
+        <v>580000</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="C11" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="D11" s="79">
-        <f>Model!I62</f>
-        <v>600000</v>
-      </c>
-      <c r="E11" s="79">
-        <f>Model!J62</f>
-        <v>930000</v>
-      </c>
-      <c r="F11" s="79">
-        <f>Model!K62</f>
-        <v>580000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" t="s">
-        <v>255</v>
-      </c>
-      <c r="C12" t="s">
-        <v>256</v>
-      </c>
-      <c r="D12" s="79">
         <f>Model!I68</f>
         <v>10000</v>
       </c>
-      <c r="E12" s="79">
+      <c r="E11" s="79">
         <f>Model!J68</f>
         <v>50000</v>
       </c>
-      <c r="F12" s="79">
+      <c r="F11" s="79">
         <f>Model!K68</f>
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B13" s="78" t="s">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B12" s="78" t="s">
         <v>280</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C12" s="85" t="s">
         <v>285</v>
       </c>
-      <c r="D13" s="86">
-        <f>D5-D8</f>
+      <c r="D12" s="86">
+        <f>D5-D7</f>
         <v>734000</v>
       </c>
-      <c r="E13" s="86">
-        <f>E5-E8</f>
+      <c r="E12" s="86">
+        <f>E5-E7</f>
         <v>831500</v>
       </c>
-      <c r="F13" s="86">
-        <f>F5-F8</f>
+      <c r="F12" s="86">
+        <f>F5-F7</f>
         <v>820000</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B14" s="60" t="s">
-        <v>257</v>
-      </c>
-      <c r="C14" s="61" t="s">
+    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="60" t="s">
+        <v>1382</v>
+      </c>
+      <c r="C13" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D14" s="64">
-        <f>SUM(D15:D20)</f>
+      <c r="D13" s="64">
+        <f>SUM(D14:D18)</f>
         <v>1217600</v>
       </c>
-      <c r="E14" s="64">
-        <f>SUM(E15:E20)</f>
+      <c r="E13" s="64">
+        <f>SUM(E14:E18)</f>
         <v>707000</v>
       </c>
-      <c r="F14" s="64">
-        <f>SUM(F15:F20)</f>
+      <c r="F13" s="64">
+        <f>SUM(F14:F18)</f>
         <v>472800</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>258</v>
+      </c>
+      <c r="C14" t="s">
+        <v>259</v>
+      </c>
+      <c r="D14" s="79">
+        <f>Model!I130</f>
+        <v>811000</v>
+      </c>
+      <c r="E14" s="79">
+        <f>Model!J130</f>
+        <v>490000</v>
+      </c>
+      <c r="F14" s="79">
+        <f>Model!K130</f>
+        <v>272500</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C15" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D15" s="79">
-        <f>Model!I130</f>
-        <v>811000</v>
+        <f>Model!I169</f>
+        <v>42100</v>
       </c>
       <c r="E15" s="79">
-        <f>Model!J130</f>
-        <v>490000</v>
+        <f>Model!J169</f>
+        <v>49500</v>
       </c>
       <c r="F15" s="79">
-        <f>Model!K130</f>
-        <v>272500</v>
+        <f>Model!K169</f>
+        <v>20300</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C16" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D16" s="79">
-        <f>Model!I169</f>
-        <v>42100</v>
+        <f>Model!I149</f>
+        <v>38000</v>
       </c>
       <c r="E16" s="79">
-        <f>Model!J169</f>
-        <v>49500</v>
+        <f>Model!J149</f>
+        <v>103500</v>
       </c>
       <c r="F16" s="79">
-        <f>Model!K169</f>
-        <v>20300</v>
+        <f>Model!K149</f>
+        <v>75000</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C17" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D17" s="79">
-        <f>Model!I149</f>
-        <v>38000</v>
+        <f>Model!I176</f>
+        <v>85000</v>
       </c>
       <c r="E17" s="79">
-        <f>Model!J149</f>
-        <v>103500</v>
+        <f>Model!J176</f>
+        <v>0</v>
       </c>
       <c r="F17" s="79">
-        <f>Model!K149</f>
-        <v>75000</v>
+        <f>Model!K176</f>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C18" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D18" s="79">
-        <f>Model!I176</f>
-        <v>85000</v>
-      </c>
-      <c r="E18" s="79">
-        <f>Model!J176</f>
-        <v>0</v>
-      </c>
-      <c r="F18" s="79">
-        <f>Model!K176</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" t="s">
-        <v>266</v>
-      </c>
-      <c r="C19" t="s">
-        <v>267</v>
-      </c>
-      <c r="D19">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <v>0</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B20" t="s">
-        <v>268</v>
-      </c>
-      <c r="C20" t="s">
-        <v>269</v>
-      </c>
-      <c r="D20" s="79">
         <f>SUM(Model!I65,Model!I71,Model!I153)</f>
         <v>241500</v>
       </c>
-      <c r="E20" s="79">
+      <c r="E18" s="79">
         <f>SUM(Model!J65,Model!J71,Model!J153)</f>
         <v>64000</v>
       </c>
-      <c r="F20" s="79">
+      <c r="F18" s="79">
         <f>SUM(Model!K65,Model!K71,Model!K153)</f>
         <v>105000</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B21" s="60" t="s">
-        <v>270</v>
-      </c>
-      <c r="C21" s="61" t="s">
-        <v>287</v>
-      </c>
-      <c r="D21" s="84">
-        <f>SUM(D22)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="84">
-        <f>SUM(E22)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="84">
-        <f>SUM(F22)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
-        <v>271</v>
-      </c>
-      <c r="C22" t="s">
-        <v>272</v>
-      </c>
-      <c r="D22">
-        <v>0</v>
-      </c>
-      <c r="E22">
-        <v>0</v>
-      </c>
-      <c r="F22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B23" s="60" t="s">
-        <v>273</v>
-      </c>
-      <c r="C23" s="61" t="s">
-        <v>288</v>
-      </c>
-      <c r="D23" s="84">
-        <f>SUM(D24:D26)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="84">
-        <f>SUM(E24:E26)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="84">
-        <f>SUM(F24:F26)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
-        <v>274</v>
-      </c>
-      <c r="C24" t="s">
-        <v>275</v>
-      </c>
-      <c r="D24">
-        <v>0</v>
-      </c>
-      <c r="E24">
-        <v>0</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>276</v>
-      </c>
-      <c r="C25" t="s">
-        <v>277</v>
-      </c>
-      <c r="D25">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B26" t="s">
-        <v>278</v>
-      </c>
-      <c r="C26" t="s">
-        <v>279</v>
-      </c>
-      <c r="D26">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B27" s="78" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="C27" s="85" t="s">
+      <c r="C19" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="D27" s="103">
-        <f>(D13-D14)+(D21-D23)</f>
+      <c r="D19" s="103">
+        <f>(D12-D13)</f>
         <v>-483600</v>
       </c>
-      <c r="E27" s="107">
-        <f>(E13-E14)+(E21-E23)</f>
+      <c r="E19" s="107">
+        <f>(E12-E13)</f>
         <v>124500</v>
       </c>
-      <c r="F27" s="107">
-        <f>(F13-F14)+(F21-F23)</f>
+      <c r="F19" s="107">
+        <f>(F12-F13)</f>
         <v>347200</v>
       </c>
     </row>
@@ -31164,7 +31793,577 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D568-367A-4BE4-A886-CC86E2F5DEA9}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="49.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="64.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>213</v>
+      </c>
+      <c r="C1" s="66" t="s">
+        <v>188</v>
+      </c>
+      <c r="D1" s="58">
+        <v>1</v>
+      </c>
+      <c r="E1" s="58">
+        <v>2</v>
+      </c>
+      <c r="F1" s="58">
+        <v>3</v>
+      </c>
+      <c r="G1" s="58">
+        <v>4</v>
+      </c>
+      <c r="H1" s="58">
+        <v>5</v>
+      </c>
+      <c r="I1" s="58">
+        <v>6</v>
+      </c>
+      <c r="J1" s="58">
+        <v>7</v>
+      </c>
+      <c r="K1" s="58">
+        <v>8</v>
+      </c>
+      <c r="L1" s="58">
+        <v>9</v>
+      </c>
+      <c r="M1" s="58">
+        <v>10</v>
+      </c>
+      <c r="N1" s="58">
+        <v>11</v>
+      </c>
+      <c r="O1" s="58">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="A2" s="54" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="66" t="s">
+        <v>215</v>
+      </c>
+      <c r="D2" s="70">
+        <v>45573</v>
+      </c>
+      <c r="E2" s="70">
+        <v>45647</v>
+      </c>
+      <c r="F2" s="70">
+        <v>45664</v>
+      </c>
+      <c r="G2" s="69"/>
+      <c r="H2" s="69"/>
+      <c r="I2" s="69"/>
+      <c r="J2" s="69"/>
+      <c r="K2" s="69"/>
+      <c r="L2" s="69"/>
+      <c r="M2" s="69"/>
+      <c r="N2" s="69"/>
+      <c r="O2" s="69"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="C3" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="D3" s="59">
+        <v>45619</v>
+      </c>
+      <c r="E3" s="59">
+        <v>45691</v>
+      </c>
+      <c r="F3" s="59">
+        <v>45705</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B4" s="53" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="53" t="s">
+        <v>167</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="E4" s="53" t="s">
+        <v>168</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B5" s="60" t="s">
+        <v>244</v>
+      </c>
+      <c r="C5" s="61" t="s">
+        <v>282</v>
+      </c>
+      <c r="D5" s="83">
+        <f>D6+D7</f>
+        <v>3266000</v>
+      </c>
+      <c r="E5" s="83">
+        <f>E6+E7</f>
+        <v>3980500</v>
+      </c>
+      <c r="F5" s="83">
+        <f>F6+F7</f>
+        <v>2870000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>245</v>
+      </c>
+      <c r="C6" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="79">
+        <f>Model!I182</f>
+        <v>3266000</v>
+      </c>
+      <c r="E6" s="79">
+        <f>Model!J182</f>
+        <v>3980500</v>
+      </c>
+      <c r="F6" s="79">
+        <f>Model!K182</f>
+        <v>2870000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>247</v>
+      </c>
+      <c r="C7" t="s">
+        <v>248</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="60" t="s">
+        <v>249</v>
+      </c>
+      <c r="C8" s="61" t="s">
+        <v>283</v>
+      </c>
+      <c r="D8" s="64">
+        <f>SUM(D9:D12)</f>
+        <v>2532000</v>
+      </c>
+      <c r="E8" s="64">
+        <f>SUM(E9:E12)</f>
+        <v>3149000</v>
+      </c>
+      <c r="F8" s="64">
+        <f>SUM(F9:F12)</f>
+        <v>2050000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
+        <v>250</v>
+      </c>
+      <c r="C9" t="s">
+        <v>284</v>
+      </c>
+      <c r="D9" s="79">
+        <f>Model!I94</f>
+        <v>1850000</v>
+      </c>
+      <c r="E9" s="79">
+        <f>Model!J94</f>
+        <v>2110000</v>
+      </c>
+      <c r="F9" s="79">
+        <f>Model!K94</f>
+        <v>1393000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>251</v>
+      </c>
+      <c r="C10" t="s">
+        <v>252</v>
+      </c>
+      <c r="D10" s="79">
+        <f>Model!I74</f>
+        <v>72000</v>
+      </c>
+      <c r="E10" s="79">
+        <f>Model!J74</f>
+        <v>59000</v>
+      </c>
+      <c r="F10" s="79">
+        <f>Model!K74</f>
+        <v>77000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>253</v>
+      </c>
+      <c r="C11" t="s">
+        <v>254</v>
+      </c>
+      <c r="D11" s="79">
+        <f>Model!I62</f>
+        <v>600000</v>
+      </c>
+      <c r="E11" s="79">
+        <f>Model!J62</f>
+        <v>930000</v>
+      </c>
+      <c r="F11" s="79">
+        <f>Model!K62</f>
+        <v>580000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>255</v>
+      </c>
+      <c r="C12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D12" s="79">
+        <f>Model!I68</f>
+        <v>10000</v>
+      </c>
+      <c r="E12" s="79">
+        <f>Model!J68</f>
+        <v>50000</v>
+      </c>
+      <c r="F12" s="79">
+        <f>Model!K68</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" s="78" t="s">
+        <v>280</v>
+      </c>
+      <c r="C13" s="85" t="s">
+        <v>285</v>
+      </c>
+      <c r="D13" s="86">
+        <f>D5-D8</f>
+        <v>734000</v>
+      </c>
+      <c r="E13" s="86">
+        <f>E5-E8</f>
+        <v>831500</v>
+      </c>
+      <c r="F13" s="86">
+        <f>F5-F8</f>
+        <v>820000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B14" s="60" t="s">
+        <v>257</v>
+      </c>
+      <c r="C14" s="61" t="s">
+        <v>281</v>
+      </c>
+      <c r="D14" s="64">
+        <f>SUM(D15:D20)</f>
+        <v>1217600</v>
+      </c>
+      <c r="E14" s="64">
+        <f>SUM(E15:E20)</f>
+        <v>707000</v>
+      </c>
+      <c r="F14" s="64">
+        <f>SUM(F15:F20)</f>
+        <v>472800</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B15" t="s">
+        <v>258</v>
+      </c>
+      <c r="C15" t="s">
+        <v>259</v>
+      </c>
+      <c r="D15" s="79">
+        <f>Model!I130</f>
+        <v>811000</v>
+      </c>
+      <c r="E15" s="79">
+        <f>Model!J130</f>
+        <v>490000</v>
+      </c>
+      <c r="F15" s="79">
+        <f>Model!K130</f>
+        <v>272500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>260</v>
+      </c>
+      <c r="C16" t="s">
+        <v>261</v>
+      </c>
+      <c r="D16" s="79">
+        <f>Model!I169</f>
+        <v>42100</v>
+      </c>
+      <c r="E16" s="79">
+        <f>Model!J169</f>
+        <v>49500</v>
+      </c>
+      <c r="F16" s="79">
+        <f>Model!K169</f>
+        <v>20300</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>262</v>
+      </c>
+      <c r="C17" t="s">
+        <v>263</v>
+      </c>
+      <c r="D17" s="79">
+        <f>Model!I149</f>
+        <v>38000</v>
+      </c>
+      <c r="E17" s="79">
+        <f>Model!J149</f>
+        <v>103500</v>
+      </c>
+      <c r="F17" s="79">
+        <f>Model!K149</f>
+        <v>75000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>264</v>
+      </c>
+      <c r="C18" t="s">
+        <v>265</v>
+      </c>
+      <c r="D18" s="79">
+        <f>Model!I176</f>
+        <v>85000</v>
+      </c>
+      <c r="E18" s="79">
+        <f>Model!J176</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="79">
+        <f>Model!K176</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>266</v>
+      </c>
+      <c r="C19" t="s">
+        <v>267</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>268</v>
+      </c>
+      <c r="C20" t="s">
+        <v>269</v>
+      </c>
+      <c r="D20" s="79">
+        <f>SUM(Model!I65,Model!I71,Model!I153)</f>
+        <v>241500</v>
+      </c>
+      <c r="E20" s="79">
+        <f>SUM(Model!J65,Model!J71,Model!J153)</f>
+        <v>64000</v>
+      </c>
+      <c r="F20" s="79">
+        <f>SUM(Model!K65,Model!K71,Model!K153)</f>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B21" s="60" t="s">
+        <v>270</v>
+      </c>
+      <c r="C21" s="61" t="s">
+        <v>287</v>
+      </c>
+      <c r="D21" s="84">
+        <f>SUM(D22)</f>
+        <v>0</v>
+      </c>
+      <c r="E21" s="84">
+        <f>SUM(E22)</f>
+        <v>0</v>
+      </c>
+      <c r="F21" s="84">
+        <f>SUM(F22)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>271</v>
+      </c>
+      <c r="C22" t="s">
+        <v>272</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B23" s="60" t="s">
+        <v>273</v>
+      </c>
+      <c r="C23" s="61" t="s">
+        <v>288</v>
+      </c>
+      <c r="D23" s="84">
+        <f>SUM(D24:D26)</f>
+        <v>0</v>
+      </c>
+      <c r="E23" s="84">
+        <f>SUM(E24:E26)</f>
+        <v>0</v>
+      </c>
+      <c r="F23" s="84">
+        <f>SUM(F24:F26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>274</v>
+      </c>
+      <c r="C24" t="s">
+        <v>275</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>276</v>
+      </c>
+      <c r="C25" t="s">
+        <v>277</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B26" t="s">
+        <v>278</v>
+      </c>
+      <c r="C26" t="s">
+        <v>279</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="78" t="s">
+        <v>286</v>
+      </c>
+      <c r="C27" s="85" t="s">
+        <v>318</v>
+      </c>
+      <c r="D27" s="103">
+        <f>(D13-D14)+(D21-D23)</f>
+        <v>-483600</v>
+      </c>
+      <c r="E27" s="107">
+        <f>(E13-E14)+(E21-E23)</f>
+        <v>124500</v>
+      </c>
+      <c r="F27" s="107">
+        <f>(F13-F14)+(F21-F23)</f>
+        <v>347200</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="54" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF553F6-B347-4C26-B8A7-42BAE6B2E22D}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -31640,7 +32839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7ADF73-DE4A-46D8-82F2-AFD0914F50C9}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -31929,7 +33128,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19143D9F-1D2E-4CB4-B765-B125ECCB2799}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -33533,7 +34732,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C455698-8A41-49C3-93EF-48D6FC05212C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -35052,7 +36251,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59C2935-E4FF-4C84-94C8-788917208325}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -36482,7 +37681,76 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE546C0-0BB7-4AA6-BB20-2385F955D524}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="126" t="s">
+        <v>512</v>
+      </c>
+      <c r="B1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="126" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E4" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>991</v>
+      </c>
+      <c r="B5">
+        <v>35000</v>
+      </c>
+      <c r="C5">
+        <v>2369000</v>
+      </c>
+      <c r="D5">
+        <v>485500</v>
+      </c>
+      <c r="E5">
+        <v>2889500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DAF883-8E55-4274-9AB3-08DD83F42302}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -37632,7 +38900,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A07A7A-3241-4130-B94F-2C4C0C305C54}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -38221,76 +39489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE546C0-0BB7-4AA6-BB20-2385F955D524}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="126" t="s">
-        <v>512</v>
-      </c>
-      <c r="B1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="126" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>581</v>
-      </c>
-      <c r="C4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E4" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>991</v>
-      </c>
-      <c r="B5">
-        <v>35000</v>
-      </c>
-      <c r="C5">
-        <v>2369000</v>
-      </c>
-      <c r="D5">
-        <v>485500</v>
-      </c>
-      <c r="E5">
-        <v>2889500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1707F40A-A58B-4C5F-AFCB-FE4A17F7D6FB}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -53578,7 +54777,7 @@
   </sheetPr>
   <dimension ref="A1:AA193"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G172" sqref="G172"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added new data 20250327
</commit_message>
<xml_diff>
--- a/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
+++ b/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Parking Lot\Web Projects\jc-farms\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06FD297C-857E-4F37-92FD-D787E5EF229E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB62A9C2-47DA-4583-89E9-77FEEE399C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="20" activeTab="22" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="17" activeTab="18" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
   </bookViews>
   <sheets>
     <sheet name="20250131 to 20250213" sheetId="15" r:id="rId1"/>
@@ -31,20 +31,21 @@
     <sheet name="Joseph_PR_20M - 27M" sheetId="29" r:id="rId16"/>
     <sheet name="Nico_PR_16M to Sale" sheetId="28" r:id="rId17"/>
     <sheet name="Nico_PR_25Mar to 8Apr" sheetId="31" r:id="rId18"/>
-    <sheet name="Template" sheetId="12" r:id="rId19"/>
-    <sheet name="&lt;&lt;&lt; Budget Forecasts" sheetId="16" r:id="rId20"/>
-    <sheet name="Detailed Financials &gt;&gt;" sheetId="17" r:id="rId21"/>
-    <sheet name="Model" sheetId="1" r:id="rId22"/>
-    <sheet name="PnL" sheetId="32" r:id="rId23"/>
-    <sheet name="P + L  Income Statement" sheetId="7" r:id="rId24"/>
-    <sheet name="Balance Sheet" sheetId="6" r:id="rId25"/>
-    <sheet name="Cash Flow Statement" sheetId="8" r:id="rId26"/>
-    <sheet name="Chicken House 2 - 300" sheetId="11" r:id="rId27"/>
-    <sheet name="Chicken House - 500" sheetId="2" r:id="rId28"/>
-    <sheet name="Guard House" sheetId="3" r:id="rId29"/>
-    <sheet name="Finishings" sheetId="4" r:id="rId30"/>
-    <sheet name="Floor and Stone Work" sheetId="5" r:id="rId31"/>
-    <sheet name="Sheet2" sheetId="18" r:id="rId32"/>
+    <sheet name="Joseph_PR_27Mar - 10Apr" sheetId="33" r:id="rId19"/>
+    <sheet name="Template" sheetId="12" r:id="rId20"/>
+    <sheet name="&lt;&lt;&lt; Budget Forecasts" sheetId="16" r:id="rId21"/>
+    <sheet name="Detailed Financials &gt;&gt;" sheetId="17" r:id="rId22"/>
+    <sheet name="Model" sheetId="1" r:id="rId23"/>
+    <sheet name="PnL" sheetId="32" r:id="rId24"/>
+    <sheet name="P + L  Income Statement" sheetId="7" r:id="rId25"/>
+    <sheet name="Balance Sheet" sheetId="6" r:id="rId26"/>
+    <sheet name="Cash Flow Statement" sheetId="8" r:id="rId27"/>
+    <sheet name="Chicken House 2 - 300" sheetId="11" r:id="rId28"/>
+    <sheet name="Chicken House - 500" sheetId="2" r:id="rId29"/>
+    <sheet name="Guard House" sheetId="3" r:id="rId30"/>
+    <sheet name="Finishings" sheetId="4" r:id="rId31"/>
+    <sheet name="Floor and Stone Work" sheetId="5" r:id="rId32"/>
+    <sheet name="Sheet2" sheetId="18" r:id="rId33"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'20250128 to 20250302'!$A$1:$AA$100</definedName>
@@ -53,7 +54,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId33"/>
+    <pivotCache cacheId="0" r:id="rId34"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -209,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7661" uniqueCount="1383">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7681" uniqueCount="1385">
   <si>
     <t>A. Capital Expenditure (Capex)</t>
   </si>
@@ -4358,6 +4359,12 @@
   </si>
   <si>
     <t>Operating Expenses (OPEX)</t>
+  </si>
+  <si>
+    <t>Transport for picking feeds and vaccination</t>
+  </si>
+  <si>
+    <t>Gombolo</t>
   </si>
 </sst>
 </file>
@@ -16060,7 +16067,7 @@
   </sheetPr>
   <dimension ref="A1:Q41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B8" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="B25" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B11" sqref="B11:N12"/>
     </sheetView>
   </sheetViews>
@@ -18252,15 +18259,15 @@
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD012E-1301-4CDB-B54B-ED7FEAC48C53}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C05BE38D-B8C6-459F-B4B9-788E1AFE0AE8}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O41"/>
+  <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -18271,14 +18278,14 @@
     <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="73" t="s">
         <v>691</v>
       </c>
       <c r="B1" s="73"/>
     </row>
-    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="E3" s="137" t="s">
         <v>225</v>
       </c>
@@ -18291,7 +18298,7 @@
       <c r="L3" s="139"/>
       <c r="N3" s="59"/>
     </row>
-    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="74" t="s">
         <v>388</v>
       </c>
@@ -18335,12 +18342,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B5" s="61" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="96"/>
       <c r="C6" s="97"/>
       <c r="D6" s="98"/>
@@ -18356,7 +18363,7 @@
       <c r="N6" s="98"/>
       <c r="O6" s="97"/>
     </row>
-    <row r="7" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="96"/>
       <c r="C7" s="97"/>
       <c r="D7" s="98"/>
@@ -18372,7 +18379,7 @@
       <c r="N7" s="98"/>
       <c r="O7" s="97"/>
     </row>
-    <row r="8" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="96"/>
       <c r="C8" s="97"/>
       <c r="D8" s="98"/>
@@ -18388,7 +18395,7 @@
       <c r="N8" s="98"/>
       <c r="O8" s="97"/>
     </row>
-    <row r="9" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="97"/>
       <c r="C9" s="97"/>
       <c r="D9" s="98"/>
@@ -18404,7 +18411,7 @@
       <c r="N9" s="98"/>
       <c r="O9" s="97"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="B10" s="61" t="s">
         <v>217</v>
       </c>
@@ -18413,39 +18420,65 @@
       <c r="F10" s="56"/>
       <c r="N10" s="56"/>
     </row>
-    <row r="11" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="96"/>
-      <c r="C11" s="97"/>
-      <c r="D11" s="98"/>
+    <row r="11" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="96" t="s">
+        <v>700</v>
+      </c>
+      <c r="C11" s="97">
+        <v>280</v>
+      </c>
+      <c r="D11" s="98">
+        <v>1500</v>
+      </c>
       <c r="E11" s="98"/>
       <c r="F11" s="97"/>
       <c r="G11" s="98"/>
-      <c r="H11" s="98"/>
+      <c r="H11" s="98">
+        <f>C11*D11</f>
+        <v>420000</v>
+      </c>
       <c r="I11" s="98"/>
       <c r="J11" s="98"/>
       <c r="K11" s="98"/>
       <c r="L11" s="98"/>
       <c r="M11" s="97"/>
-      <c r="N11" s="98"/>
+      <c r="N11" s="98">
+        <f>H11</f>
+        <v>420000</v>
+      </c>
       <c r="O11" s="97"/>
-    </row>
-    <row r="12" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="96"/>
-      <c r="C12" s="97"/>
-      <c r="D12" s="98"/>
+      <c r="P11" s="136"/>
+    </row>
+    <row r="12" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="96" t="s">
+        <v>1124</v>
+      </c>
+      <c r="C12" s="97">
+        <v>100</v>
+      </c>
+      <c r="D12" s="98">
+        <v>4300</v>
+      </c>
       <c r="E12" s="98"/>
       <c r="F12" s="99"/>
       <c r="G12" s="98"/>
-      <c r="H12" s="98"/>
+      <c r="H12" s="98">
+        <f>C12*D12</f>
+        <v>430000</v>
+      </c>
       <c r="I12" s="98"/>
       <c r="J12" s="98"/>
       <c r="K12" s="98"/>
       <c r="L12" s="98"/>
       <c r="M12" s="97"/>
-      <c r="N12" s="98"/>
+      <c r="N12" s="98">
+        <f>H12</f>
+        <v>430000</v>
+      </c>
       <c r="O12" s="97"/>
-    </row>
-    <row r="13" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="79"/>
+    </row>
+    <row r="13" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="96"/>
       <c r="C13" s="97"/>
       <c r="D13" s="98"/>
@@ -18461,7 +18494,7 @@
       <c r="N13" s="98"/>
       <c r="O13" s="97"/>
     </row>
-    <row r="14" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="96"/>
       <c r="C14" s="97"/>
       <c r="D14" s="98"/>
@@ -18477,7 +18510,7 @@
       <c r="N14" s="98"/>
       <c r="O14" s="97"/>
     </row>
-    <row r="15" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="96"/>
       <c r="C15" s="97"/>
       <c r="D15" s="98"/>
@@ -18493,7 +18526,7 @@
       <c r="N15" s="98"/>
       <c r="O15" s="97"/>
     </row>
-    <row r="16" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="96"/>
       <c r="C16" s="97"/>
       <c r="D16" s="98"/>
@@ -18509,7 +18542,7 @@
       <c r="N16" s="98"/>
       <c r="O16" s="97"/>
     </row>
-    <row r="17" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="96"/>
       <c r="C17" s="97"/>
       <c r="D17" s="98"/>
@@ -18525,7 +18558,7 @@
       <c r="N17" s="98"/>
       <c r="O17" s="97"/>
     </row>
-    <row r="18" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="96"/>
       <c r="C18" s="97"/>
       <c r="D18" s="98"/>
@@ -18541,7 +18574,7 @@
       <c r="N18" s="98"/>
       <c r="O18" s="97"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B19" s="71" t="s">
         <v>113</v>
       </c>
@@ -18550,23 +18583,36 @@
       <c r="F19" s="56"/>
       <c r="N19" s="56"/>
     </row>
-    <row r="20" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="96"/>
-      <c r="C20" s="97"/>
-      <c r="D20" s="98"/>
+    <row r="20" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="96" t="s">
+        <v>1383</v>
+      </c>
+      <c r="C20" s="97">
+        <v>2</v>
+      </c>
+      <c r="D20" s="98">
+        <v>10000</v>
+      </c>
       <c r="E20" s="98"/>
       <c r="F20" s="98"/>
       <c r="G20" s="97"/>
-      <c r="H20" s="97"/>
+      <c r="H20" s="99">
+        <f>C20*D20</f>
+        <v>20000</v>
+      </c>
       <c r="I20" s="97"/>
       <c r="J20" s="97"/>
       <c r="K20" s="97"/>
       <c r="L20" s="97"/>
       <c r="M20" s="97"/>
-      <c r="N20" s="98"/>
+      <c r="N20" s="98">
+        <f>H20</f>
+        <v>20000</v>
+      </c>
       <c r="O20" s="97"/>
-    </row>
-    <row r="21" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P20" s="79"/>
+    </row>
+    <row r="21" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="96"/>
       <c r="C21" s="97"/>
       <c r="D21" s="98"/>
@@ -18582,7 +18628,7 @@
       <c r="N21" s="98"/>
       <c r="O21" s="97"/>
     </row>
-    <row r="22" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="96"/>
       <c r="C22" s="97"/>
       <c r="D22" s="98"/>
@@ -18598,7 +18644,7 @@
       <c r="N22" s="98"/>
       <c r="O22" s="97"/>
     </row>
-    <row r="23" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="96"/>
       <c r="C23" s="97"/>
       <c r="D23" s="98"/>
@@ -18614,7 +18660,7 @@
       <c r="N23" s="98"/>
       <c r="O23" s="97"/>
     </row>
-    <row r="24" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="96"/>
       <c r="C24" s="97"/>
       <c r="D24" s="98"/>
@@ -18630,7 +18676,7 @@
       <c r="N24" s="98"/>
       <c r="O24" s="97"/>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B25" s="71" t="s">
         <v>368</v>
       </c>
@@ -18639,30 +18685,43 @@
       <c r="F25" s="56"/>
       <c r="N25" s="56"/>
     </row>
-    <row r="26" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B26" s="96"/>
-      <c r="C26" s="97"/>
-      <c r="D26" s="98"/>
+    <row r="26" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="96" t="s">
+        <v>1384</v>
+      </c>
+      <c r="C26" s="97">
+        <v>500</v>
+      </c>
+      <c r="D26" s="98">
+        <v>24</v>
+      </c>
       <c r="E26" s="97"/>
       <c r="F26" s="98"/>
       <c r="G26" s="97"/>
-      <c r="H26" s="97"/>
+      <c r="H26" s="99">
+        <f>C26*D26</f>
+        <v>12000</v>
+      </c>
       <c r="I26" s="97"/>
       <c r="J26" s="97"/>
       <c r="K26" s="97"/>
       <c r="L26" s="97"/>
       <c r="M26" s="97"/>
-      <c r="N26" s="100"/>
+      <c r="N26" s="100">
+        <f>H26</f>
+        <v>12000</v>
+      </c>
       <c r="O26" s="97"/>
-    </row>
-    <row r="27" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P26" s="79"/>
+    </row>
+    <row r="27" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="96"/>
       <c r="C27" s="97"/>
       <c r="D27" s="98"/>
       <c r="E27" s="97"/>
       <c r="F27" s="98"/>
       <c r="G27" s="97"/>
-      <c r="H27" s="97"/>
+      <c r="H27" s="99"/>
       <c r="I27" s="97"/>
       <c r="J27" s="97"/>
       <c r="K27" s="97"/>
@@ -18670,24 +18729,26 @@
       <c r="M27" s="97"/>
       <c r="N27" s="100"/>
       <c r="O27" s="97"/>
-    </row>
-    <row r="28" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="96"/>
-      <c r="C28" s="97"/>
-      <c r="D28" s="98"/>
-      <c r="E28" s="97"/>
-      <c r="F28" s="98"/>
-      <c r="G28" s="97"/>
-      <c r="H28" s="97"/>
-      <c r="I28" s="97"/>
+      <c r="P27" s="79"/>
+    </row>
+    <row r="28" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="110"/>
+      <c r="C28" s="111"/>
+      <c r="D28" s="112"/>
+      <c r="E28" s="111"/>
+      <c r="F28" s="112"/>
+      <c r="G28" s="111"/>
+      <c r="H28" s="111"/>
+      <c r="I28" s="113"/>
       <c r="J28" s="97"/>
       <c r="K28" s="97"/>
       <c r="L28" s="97"/>
-      <c r="M28" s="97"/>
-      <c r="N28" s="100"/>
-      <c r="O28" s="97"/>
-    </row>
-    <row r="29" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="M28" s="111"/>
+      <c r="N28" s="114"/>
+      <c r="O28" s="113"/>
+      <c r="P28" s="136"/>
+    </row>
+    <row r="29" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="96"/>
       <c r="C29" s="97"/>
       <c r="D29" s="98"/>
@@ -18703,7 +18764,7 @@
       <c r="N29" s="100"/>
       <c r="O29" s="97"/>
     </row>
-    <row r="30" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="96"/>
       <c r="C30" s="97"/>
       <c r="D30" s="98"/>
@@ -18719,7 +18780,7 @@
       <c r="N30" s="100"/>
       <c r="O30" s="97"/>
     </row>
-    <row r="31" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B31" s="96"/>
       <c r="C31" s="97"/>
       <c r="D31" s="98"/>
@@ -18735,7 +18796,7 @@
       <c r="N31" s="100"/>
       <c r="O31" s="97"/>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B32" s="71" t="s">
         <v>227</v>
       </c>
@@ -18744,7 +18805,7 @@
       <c r="F32" s="56"/>
       <c r="N32" s="56"/>
     </row>
-    <row r="33" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B33" s="96"/>
       <c r="C33" s="97"/>
       <c r="D33" s="98"/>
@@ -18760,7 +18821,7 @@
       <c r="N33" s="98"/>
       <c r="O33" s="97"/>
     </row>
-    <row r="34" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B34" s="96"/>
       <c r="C34" s="97"/>
       <c r="D34" s="98"/>
@@ -18776,7 +18837,7 @@
       <c r="N34" s="98"/>
       <c r="O34" s="97"/>
     </row>
-    <row r="35" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B35" s="96"/>
       <c r="C35" s="97"/>
       <c r="D35" s="98"/>
@@ -18792,16 +18853,22 @@
       <c r="N35" s="98"/>
       <c r="O35" s="97"/>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+    <row r="36" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B36" s="61" t="s">
-        <v>237</v>
+        <v>696</v>
       </c>
       <c r="N36" s="56"/>
     </row>
-    <row r="37" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="96"/>
-      <c r="C37" s="97"/>
-      <c r="D37" s="97"/>
+    <row r="37" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="96" t="s">
+        <v>331</v>
+      </c>
+      <c r="C37" s="97">
+        <v>1</v>
+      </c>
+      <c r="D37" s="97">
+        <v>18000</v>
+      </c>
       <c r="E37" s="97"/>
       <c r="F37" s="97"/>
       <c r="G37" s="97"/>
@@ -18811,10 +18878,14 @@
       <c r="K37" s="97"/>
       <c r="L37" s="97"/>
       <c r="M37" s="97"/>
-      <c r="N37" s="98"/>
+      <c r="N37" s="98">
+        <f>D37</f>
+        <v>18000</v>
+      </c>
       <c r="O37" s="97"/>
-    </row>
-    <row r="38" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P37" s="79"/>
+    </row>
+    <row r="38" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B38" s="96"/>
       <c r="C38" s="97"/>
       <c r="D38" s="97"/>
@@ -18830,7 +18901,7 @@
       <c r="N38" s="98"/>
       <c r="O38" s="97"/>
     </row>
-    <row r="39" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:16" ht="25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B39" s="97"/>
       <c r="C39" s="97"/>
       <c r="D39" s="97"/>
@@ -18846,7 +18917,7 @@
       <c r="N39" s="98"/>
       <c r="O39" s="97"/>
     </row>
-    <row r="40" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="40" spans="2:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B40" s="72"/>
       <c r="C40" s="72"/>
       <c r="D40" s="72"/>
@@ -18862,11 +18933,13 @@
         <v>234</v>
       </c>
       <c r="N40" s="102">
-        <f>SUM(N5:N36)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+        <f>SUM(N5:N37)</f>
+        <v>900000</v>
+      </c>
+      <c r="O40" s="102"/>
+      <c r="P40" s="79"/>
+    </row>
+    <row r="41" spans="2:16" x14ac:dyDescent="0.35">
       <c r="N41" s="56"/>
     </row>
   </sheetData>
@@ -21918,6 +21991,633 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5FD012E-1301-4CDB-B54B-ED7FEAC48C53}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:O41"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A28" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="45" bestFit="1" customWidth="1"/>
+    <col min="3" max="12" width="10.7265625" customWidth="1"/>
+    <col min="13" max="13" width="36.54296875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="73" t="s">
+        <v>691</v>
+      </c>
+      <c r="B1" s="73"/>
+    </row>
+    <row r="2" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="E3" s="137" t="s">
+        <v>225</v>
+      </c>
+      <c r="F3" s="138"/>
+      <c r="G3" s="138"/>
+      <c r="H3" s="138"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="139"/>
+      <c r="N3" s="59"/>
+    </row>
+    <row r="4" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B4" s="74" t="s">
+        <v>388</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="74" t="s">
+        <v>219</v>
+      </c>
+      <c r="E4" s="105">
+        <v>4</v>
+      </c>
+      <c r="F4" s="105">
+        <v>5</v>
+      </c>
+      <c r="G4" s="105">
+        <v>6</v>
+      </c>
+      <c r="H4" s="105">
+        <v>7</v>
+      </c>
+      <c r="I4" s="105">
+        <v>8</v>
+      </c>
+      <c r="J4" s="105">
+        <v>9</v>
+      </c>
+      <c r="K4" s="105">
+        <v>10</v>
+      </c>
+      <c r="L4" s="105">
+        <v>11</v>
+      </c>
+      <c r="M4" s="74" t="s">
+        <v>104</v>
+      </c>
+      <c r="N4" s="74" t="s">
+        <v>233</v>
+      </c>
+      <c r="O4" s="74" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B5" s="61" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="96"/>
+      <c r="C6" s="97"/>
+      <c r="D6" s="98"/>
+      <c r="E6" s="98"/>
+      <c r="F6" s="98"/>
+      <c r="G6" s="99"/>
+      <c r="H6" s="99"/>
+      <c r="I6" s="99"/>
+      <c r="J6" s="99"/>
+      <c r="K6" s="99"/>
+      <c r="L6" s="99"/>
+      <c r="M6" s="97"/>
+      <c r="N6" s="98"/>
+      <c r="O6" s="97"/>
+    </row>
+    <row r="7" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="98"/>
+      <c r="E7" s="98"/>
+      <c r="F7" s="98"/>
+      <c r="G7" s="99"/>
+      <c r="H7" s="99"/>
+      <c r="I7" s="99"/>
+      <c r="J7" s="99"/>
+      <c r="K7" s="99"/>
+      <c r="L7" s="99"/>
+      <c r="M7" s="97"/>
+      <c r="N7" s="98"/>
+      <c r="O7" s="97"/>
+    </row>
+    <row r="8" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="96"/>
+      <c r="C8" s="97"/>
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+      <c r="F8" s="98"/>
+      <c r="G8" s="99"/>
+      <c r="H8" s="99"/>
+      <c r="I8" s="99"/>
+      <c r="J8" s="99"/>
+      <c r="K8" s="99"/>
+      <c r="L8" s="99"/>
+      <c r="M8" s="97"/>
+      <c r="N8" s="98"/>
+      <c r="O8" s="97"/>
+    </row>
+    <row r="9" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="97"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="98"/>
+      <c r="E9" s="98"/>
+      <c r="F9" s="98"/>
+      <c r="G9" s="97"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="97"/>
+      <c r="M9" s="97"/>
+      <c r="N9" s="98"/>
+      <c r="O9" s="97"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B10" s="61" t="s">
+        <v>217</v>
+      </c>
+      <c r="D10" s="56"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="56"/>
+      <c r="N10" s="56"/>
+    </row>
+    <row r="11" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="98"/>
+      <c r="E11" s="98"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="98"/>
+      <c r="H11" s="98"/>
+      <c r="I11" s="98"/>
+      <c r="J11" s="98"/>
+      <c r="K11" s="98"/>
+      <c r="L11" s="98"/>
+      <c r="M11" s="97"/>
+      <c r="N11" s="98"/>
+      <c r="O11" s="97"/>
+    </row>
+    <row r="12" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B12" s="96"/>
+      <c r="C12" s="97"/>
+      <c r="D12" s="98"/>
+      <c r="E12" s="98"/>
+      <c r="F12" s="99"/>
+      <c r="G12" s="98"/>
+      <c r="H12" s="98"/>
+      <c r="I12" s="98"/>
+      <c r="J12" s="98"/>
+      <c r="K12" s="98"/>
+      <c r="L12" s="98"/>
+      <c r="M12" s="97"/>
+      <c r="N12" s="98"/>
+      <c r="O12" s="97"/>
+    </row>
+    <row r="13" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="96"/>
+      <c r="C13" s="97"/>
+      <c r="D13" s="98"/>
+      <c r="E13" s="97"/>
+      <c r="F13" s="98"/>
+      <c r="G13" s="97"/>
+      <c r="H13" s="97"/>
+      <c r="I13" s="97"/>
+      <c r="J13" s="97"/>
+      <c r="K13" s="97"/>
+      <c r="L13" s="97"/>
+      <c r="M13" s="97"/>
+      <c r="N13" s="98"/>
+      <c r="O13" s="97"/>
+    </row>
+    <row r="14" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="96"/>
+      <c r="C14" s="97"/>
+      <c r="D14" s="98"/>
+      <c r="E14" s="97"/>
+      <c r="F14" s="98"/>
+      <c r="G14" s="97"/>
+      <c r="H14" s="97"/>
+      <c r="I14" s="97"/>
+      <c r="J14" s="97"/>
+      <c r="K14" s="97"/>
+      <c r="L14" s="97"/>
+      <c r="M14" s="97"/>
+      <c r="N14" s="98"/>
+      <c r="O14" s="97"/>
+    </row>
+    <row r="15" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B15" s="96"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="98"/>
+      <c r="E15" s="98"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="98"/>
+      <c r="H15" s="98"/>
+      <c r="I15" s="98"/>
+      <c r="J15" s="98"/>
+      <c r="K15" s="98"/>
+      <c r="L15" s="98"/>
+      <c r="M15" s="97"/>
+      <c r="N15" s="98"/>
+      <c r="O15" s="97"/>
+    </row>
+    <row r="16" spans="1:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B16" s="96"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="98"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="98"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="I16" s="97"/>
+      <c r="J16" s="97"/>
+      <c r="K16" s="97"/>
+      <c r="L16" s="97"/>
+      <c r="M16" s="97"/>
+      <c r="N16" s="98"/>
+      <c r="O16" s="97"/>
+    </row>
+    <row r="17" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B17" s="96"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="98"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="98"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
+      <c r="I17" s="97"/>
+      <c r="J17" s="97"/>
+      <c r="K17" s="97"/>
+      <c r="L17" s="97"/>
+      <c r="M17" s="97"/>
+      <c r="N17" s="98"/>
+      <c r="O17" s="97"/>
+    </row>
+    <row r="18" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B18" s="96"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="98"/>
+      <c r="E18" s="98"/>
+      <c r="F18" s="98"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
+      <c r="I18" s="97"/>
+      <c r="J18" s="97"/>
+      <c r="K18" s="97"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="97"/>
+      <c r="N18" s="98"/>
+      <c r="O18" s="97"/>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B19" s="71" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
+      <c r="N19" s="56"/>
+    </row>
+    <row r="20" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B20" s="96"/>
+      <c r="C20" s="97"/>
+      <c r="D20" s="98"/>
+      <c r="E20" s="98"/>
+      <c r="F20" s="98"/>
+      <c r="G20" s="97"/>
+      <c r="H20" s="97"/>
+      <c r="I20" s="97"/>
+      <c r="J20" s="97"/>
+      <c r="K20" s="97"/>
+      <c r="L20" s="97"/>
+      <c r="M20" s="97"/>
+      <c r="N20" s="98"/>
+      <c r="O20" s="97"/>
+    </row>
+    <row r="21" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B21" s="96"/>
+      <c r="C21" s="97"/>
+      <c r="D21" s="98"/>
+      <c r="E21" s="98"/>
+      <c r="F21" s="98"/>
+      <c r="G21" s="97"/>
+      <c r="H21" s="97"/>
+      <c r="I21" s="97"/>
+      <c r="J21" s="97"/>
+      <c r="K21" s="97"/>
+      <c r="L21" s="97"/>
+      <c r="M21" s="97"/>
+      <c r="N21" s="98"/>
+      <c r="O21" s="97"/>
+    </row>
+    <row r="22" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B22" s="96"/>
+      <c r="C22" s="97"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="97"/>
+      <c r="H22" s="97"/>
+      <c r="I22" s="97"/>
+      <c r="J22" s="97"/>
+      <c r="K22" s="97"/>
+      <c r="L22" s="97"/>
+      <c r="M22" s="97"/>
+      <c r="N22" s="98"/>
+      <c r="O22" s="97"/>
+    </row>
+    <row r="23" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B23" s="96"/>
+      <c r="C23" s="97"/>
+      <c r="D23" s="98"/>
+      <c r="E23" s="98"/>
+      <c r="F23" s="98"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="99"/>
+      <c r="L23" s="99"/>
+      <c r="M23" s="97"/>
+      <c r="N23" s="98"/>
+      <c r="O23" s="97"/>
+    </row>
+    <row r="24" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B24" s="96"/>
+      <c r="C24" s="97"/>
+      <c r="D24" s="98"/>
+      <c r="E24" s="98"/>
+      <c r="F24" s="98"/>
+      <c r="G24" s="97"/>
+      <c r="H24" s="97"/>
+      <c r="I24" s="97"/>
+      <c r="J24" s="97"/>
+      <c r="K24" s="97"/>
+      <c r="L24" s="97"/>
+      <c r="M24" s="97"/>
+      <c r="N24" s="98"/>
+      <c r="O24" s="97"/>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B25" s="71" t="s">
+        <v>368</v>
+      </c>
+      <c r="D25" s="56"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="56"/>
+      <c r="N25" s="56"/>
+    </row>
+    <row r="26" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B26" s="96"/>
+      <c r="C26" s="97"/>
+      <c r="D26" s="98"/>
+      <c r="E26" s="97"/>
+      <c r="F26" s="98"/>
+      <c r="G26" s="97"/>
+      <c r="H26" s="97"/>
+      <c r="I26" s="97"/>
+      <c r="J26" s="97"/>
+      <c r="K26" s="97"/>
+      <c r="L26" s="97"/>
+      <c r="M26" s="97"/>
+      <c r="N26" s="100"/>
+      <c r="O26" s="97"/>
+    </row>
+    <row r="27" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B27" s="96"/>
+      <c r="C27" s="97"/>
+      <c r="D27" s="98"/>
+      <c r="E27" s="97"/>
+      <c r="F27" s="98"/>
+      <c r="G27" s="97"/>
+      <c r="H27" s="97"/>
+      <c r="I27" s="97"/>
+      <c r="J27" s="97"/>
+      <c r="K27" s="97"/>
+      <c r="L27" s="97"/>
+      <c r="M27" s="97"/>
+      <c r="N27" s="100"/>
+      <c r="O27" s="97"/>
+    </row>
+    <row r="28" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B28" s="96"/>
+      <c r="C28" s="97"/>
+      <c r="D28" s="98"/>
+      <c r="E28" s="97"/>
+      <c r="F28" s="98"/>
+      <c r="G28" s="97"/>
+      <c r="H28" s="97"/>
+      <c r="I28" s="97"/>
+      <c r="J28" s="97"/>
+      <c r="K28" s="97"/>
+      <c r="L28" s="97"/>
+      <c r="M28" s="97"/>
+      <c r="N28" s="100"/>
+      <c r="O28" s="97"/>
+    </row>
+    <row r="29" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B29" s="96"/>
+      <c r="C29" s="97"/>
+      <c r="D29" s="98"/>
+      <c r="E29" s="97"/>
+      <c r="F29" s="98"/>
+      <c r="G29" s="97"/>
+      <c r="H29" s="97"/>
+      <c r="I29" s="97"/>
+      <c r="J29" s="97"/>
+      <c r="K29" s="97"/>
+      <c r="L29" s="97"/>
+      <c r="M29" s="97"/>
+      <c r="N29" s="100"/>
+      <c r="O29" s="97"/>
+    </row>
+    <row r="30" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B30" s="96"/>
+      <c r="C30" s="97"/>
+      <c r="D30" s="98"/>
+      <c r="E30" s="98"/>
+      <c r="F30" s="98"/>
+      <c r="G30" s="99"/>
+      <c r="H30" s="99"/>
+      <c r="I30" s="99"/>
+      <c r="J30" s="99"/>
+      <c r="K30" s="99"/>
+      <c r="L30" s="99"/>
+      <c r="M30" s="97"/>
+      <c r="N30" s="100"/>
+      <c r="O30" s="97"/>
+    </row>
+    <row r="31" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B31" s="96"/>
+      <c r="C31" s="97"/>
+      <c r="D31" s="98"/>
+      <c r="E31" s="98"/>
+      <c r="F31" s="98"/>
+      <c r="G31" s="97"/>
+      <c r="H31" s="97"/>
+      <c r="I31" s="97"/>
+      <c r="J31" s="97"/>
+      <c r="K31" s="97"/>
+      <c r="L31" s="97"/>
+      <c r="M31" s="97"/>
+      <c r="N31" s="100"/>
+      <c r="O31" s="97"/>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B32" s="71" t="s">
+        <v>227</v>
+      </c>
+      <c r="D32" s="56"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="56"/>
+      <c r="N32" s="56"/>
+    </row>
+    <row r="33" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B33" s="96"/>
+      <c r="C33" s="97"/>
+      <c r="D33" s="98"/>
+      <c r="E33" s="98"/>
+      <c r="F33" s="98"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="97"/>
+      <c r="J33" s="97"/>
+      <c r="K33" s="97"/>
+      <c r="L33" s="97"/>
+      <c r="M33" s="97"/>
+      <c r="N33" s="98"/>
+      <c r="O33" s="97"/>
+    </row>
+    <row r="34" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B34" s="96"/>
+      <c r="C34" s="97"/>
+      <c r="D34" s="98"/>
+      <c r="E34" s="98"/>
+      <c r="F34" s="98"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="97"/>
+      <c r="K34" s="97"/>
+      <c r="L34" s="97"/>
+      <c r="M34" s="97"/>
+      <c r="N34" s="98"/>
+      <c r="O34" s="97"/>
+    </row>
+    <row r="35" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B35" s="96"/>
+      <c r="C35" s="97"/>
+      <c r="D35" s="98"/>
+      <c r="E35" s="98"/>
+      <c r="F35" s="98"/>
+      <c r="G35" s="97"/>
+      <c r="H35" s="97"/>
+      <c r="I35" s="97"/>
+      <c r="J35" s="97"/>
+      <c r="K35" s="97"/>
+      <c r="L35" s="97"/>
+      <c r="M35" s="97"/>
+      <c r="N35" s="98"/>
+      <c r="O35" s="97"/>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="B36" s="61" t="s">
+        <v>237</v>
+      </c>
+      <c r="N36" s="56"/>
+    </row>
+    <row r="37" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B37" s="96"/>
+      <c r="C37" s="97"/>
+      <c r="D37" s="97"/>
+      <c r="E37" s="97"/>
+      <c r="F37" s="97"/>
+      <c r="G37" s="97"/>
+      <c r="H37" s="97"/>
+      <c r="I37" s="97"/>
+      <c r="J37" s="97"/>
+      <c r="K37" s="97"/>
+      <c r="L37" s="97"/>
+      <c r="M37" s="97"/>
+      <c r="N37" s="98"/>
+      <c r="O37" s="97"/>
+    </row>
+    <row r="38" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B38" s="96"/>
+      <c r="C38" s="97"/>
+      <c r="D38" s="97"/>
+      <c r="E38" s="97"/>
+      <c r="F38" s="97"/>
+      <c r="G38" s="97"/>
+      <c r="H38" s="97"/>
+      <c r="I38" s="97"/>
+      <c r="J38" s="97"/>
+      <c r="K38" s="97"/>
+      <c r="L38" s="97"/>
+      <c r="M38" s="97"/>
+      <c r="N38" s="98"/>
+      <c r="O38" s="97"/>
+    </row>
+    <row r="39" spans="2:15" ht="25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B39" s="97"/>
+      <c r="C39" s="97"/>
+      <c r="D39" s="97"/>
+      <c r="E39" s="97"/>
+      <c r="F39" s="97"/>
+      <c r="G39" s="97"/>
+      <c r="H39" s="97"/>
+      <c r="I39" s="97"/>
+      <c r="J39" s="97"/>
+      <c r="K39" s="97"/>
+      <c r="L39" s="97"/>
+      <c r="M39" s="97"/>
+      <c r="N39" s="98"/>
+      <c r="O39" s="97"/>
+    </row>
+    <row r="40" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B40" s="72"/>
+      <c r="C40" s="72"/>
+      <c r="D40" s="72"/>
+      <c r="E40" s="72"/>
+      <c r="F40" s="72"/>
+      <c r="G40" s="72"/>
+      <c r="H40" s="72"/>
+      <c r="I40" s="72"/>
+      <c r="J40" s="72"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="72"/>
+      <c r="M40" s="101" t="s">
+        <v>234</v>
+      </c>
+      <c r="N40" s="102">
+        <f>SUM(N5:N36)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
+      <c r="N41" s="56"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="E3:L3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="56" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B905C8F-AA7B-4366-ACBD-214566A869AE}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -21934,7 +22634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E000CEC5-651A-41CF-9370-A65672278D0D}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -21951,7 +22651,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A94399-3FA4-4BC1-8ACB-AC4F9CB00833}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -31365,7 +32065,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B979F449-628E-4A37-A375-770828AACAA5}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -31373,8 +32073,8 @@
   </sheetPr>
   <dimension ref="A1:O19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -31793,7 +32493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B617D568-367A-4BE4-A886-CC86E2F5DEA9}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -32363,7 +33063,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BF553F6-B347-4C26-B8A7-42BAE6B2E22D}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -32839,7 +33539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF7ADF73-DE4A-46D8-82F2-AFD0914F50C9}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
@@ -33128,7 +33828,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19143D9F-1D2E-4CB4-B765-B125ECCB2799}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -34732,7 +35432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C455698-8A41-49C3-93EF-48D6FC05212C}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -36251,7 +36951,76 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE546C0-0BB7-4AA6-BB20-2385F955D524}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:E5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="126" t="s">
+        <v>512</v>
+      </c>
+      <c r="B1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B3" s="126" t="s">
+        <v>990</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>581</v>
+      </c>
+      <c r="C4" t="s">
+        <v>249</v>
+      </c>
+      <c r="D4" t="s">
+        <v>558</v>
+      </c>
+      <c r="E4" t="s">
+        <v>989</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>991</v>
+      </c>
+      <c r="B5">
+        <v>35000</v>
+      </c>
+      <c r="C5">
+        <v>2369000</v>
+      </c>
+      <c r="D5">
+        <v>485500</v>
+      </c>
+      <c r="E5">
+        <v>2889500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A59C2935-E4FF-4C84-94C8-788917208325}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -37681,76 +38450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE546C0-0BB7-4AA6-BB20-2385F955D524}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1796875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="10.7265625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A1" s="126" t="s">
-        <v>512</v>
-      </c>
-      <c r="B1" t="s">
-        <v>540</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B3" s="126" t="s">
-        <v>990</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="B4" t="s">
-        <v>581</v>
-      </c>
-      <c r="C4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D4" t="s">
-        <v>558</v>
-      </c>
-      <c r="E4" t="s">
-        <v>989</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>991</v>
-      </c>
-      <c r="B5">
-        <v>35000</v>
-      </c>
-      <c r="C5">
-        <v>2369000</v>
-      </c>
-      <c r="D5">
-        <v>485500</v>
-      </c>
-      <c r="E5">
-        <v>2889500</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33DAF883-8E55-4274-9AB3-08DD83F42302}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -38900,7 +39600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8A07A7A-3241-4130-B94F-2C4C0C305C54}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -39489,7 +40189,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1707F40A-A58B-4C5F-AFCB-FE4A17F7D6FB}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added PnL statement for batch 1 2 and 3
</commit_message>
<xml_diff>
--- a/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
+++ b/R/data/JC Poultry Farm - Business Operating Model_v1_250323.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Desktop\Parking Lot\Web Projects\jc-farms\R\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB62A9C2-47DA-4583-89E9-77FEEE399C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B554A30-B10A-4A29-A514-D48E43C1510C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="17" activeTab="18" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="20" activeTab="23" xr2:uid="{7B0A1020-A1E3-46BF-A415-695171A71206}"/>
   </bookViews>
   <sheets>
     <sheet name="20250131 to 20250213" sheetId="15" r:id="rId1"/>
@@ -210,7 +210,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7681" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7679" uniqueCount="1385">
   <si>
     <t>A. Capital Expenditure (Capex)</t>
   </si>
@@ -18266,7 +18266,7 @@
   </sheetPr>
   <dimension ref="A1:P41"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A29" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="N38" sqref="N38"/>
     </sheetView>
   </sheetViews>
@@ -32071,10 +32071,10 @@
     <tabColor rgb="FF0070C0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O19"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -32327,163 +32327,143 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="B12" s="78" t="s">
-        <v>280</v>
-      </c>
-      <c r="C12" s="85" t="s">
-        <v>285</v>
-      </c>
-      <c r="D12" s="86">
-        <f>D5-D7</f>
-        <v>734000</v>
-      </c>
-      <c r="E12" s="86">
-        <f>E5-E7</f>
-        <v>831500</v>
-      </c>
-      <c r="F12" s="86">
-        <f>F5-F7</f>
-        <v>820000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B13" s="60" t="s">
+    <row r="12" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B12" s="60" t="s">
         <v>1382</v>
       </c>
-      <c r="C13" s="61" t="s">
+      <c r="C12" s="61" t="s">
         <v>281</v>
       </c>
-      <c r="D13" s="64">
-        <f>SUM(D14:D18)</f>
+      <c r="D12" s="64">
+        <f>SUM(D13:D17)</f>
         <v>1217600</v>
       </c>
-      <c r="E13" s="64">
-        <f>SUM(E14:E18)</f>
+      <c r="E12" s="64">
+        <f>SUM(E13:E17)</f>
         <v>707000</v>
       </c>
-      <c r="F13" s="64">
-        <f>SUM(F14:F18)</f>
+      <c r="F12" s="64">
+        <f>SUM(F13:F17)</f>
         <v>472800</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>258</v>
+      </c>
+      <c r="C13" t="s">
+        <v>259</v>
+      </c>
+      <c r="D13" s="79">
+        <f>Model!I130</f>
+        <v>811000</v>
+      </c>
+      <c r="E13" s="79">
+        <f>Model!J130</f>
+        <v>490000</v>
+      </c>
+      <c r="F13" s="79">
+        <f>Model!K130</f>
+        <v>272500</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="C14" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="D14" s="79">
-        <f>Model!I130</f>
-        <v>811000</v>
+        <f>Model!I169</f>
+        <v>42100</v>
       </c>
       <c r="E14" s="79">
-        <f>Model!J130</f>
-        <v>490000</v>
+        <f>Model!J169</f>
+        <v>49500</v>
       </c>
       <c r="F14" s="79">
-        <f>Model!K130</f>
-        <v>272500</v>
+        <f>Model!K169</f>
+        <v>20300</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C15" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="D15" s="79">
-        <f>Model!I169</f>
-        <v>42100</v>
+        <f>Model!I149</f>
+        <v>38000</v>
       </c>
       <c r="E15" s="79">
-        <f>Model!J169</f>
-        <v>49500</v>
+        <f>Model!J149</f>
+        <v>103500</v>
       </c>
       <c r="F15" s="79">
-        <f>Model!K169</f>
-        <v>20300</v>
+        <f>Model!K149</f>
+        <v>75000</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C16" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="D16" s="79">
-        <f>Model!I149</f>
-        <v>38000</v>
+        <f>Model!I176</f>
+        <v>85000</v>
       </c>
       <c r="E16" s="79">
-        <f>Model!J149</f>
-        <v>103500</v>
+        <f>Model!J176</f>
+        <v>0</v>
       </c>
       <c r="F16" s="79">
-        <f>Model!K149</f>
-        <v>75000</v>
+        <f>Model!K176</f>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="C17" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="D17" s="79">
-        <f>Model!I176</f>
-        <v>85000</v>
-      </c>
-      <c r="E17" s="79">
-        <f>Model!J176</f>
-        <v>0</v>
-      </c>
-      <c r="F17" s="79">
-        <f>Model!K176</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B18" t="s">
-        <v>268</v>
-      </c>
-      <c r="C18" t="s">
-        <v>269</v>
-      </c>
-      <c r="D18" s="79">
         <f>SUM(Model!I65,Model!I71,Model!I153)</f>
         <v>241500</v>
       </c>
-      <c r="E18" s="79">
+      <c r="E17" s="79">
         <f>SUM(Model!J65,Model!J71,Model!J153)</f>
         <v>64000</v>
       </c>
-      <c r="F18" s="79">
+      <c r="F17" s="79">
         <f>SUM(Model!K65,Model!K71,Model!K153)</f>
         <v>105000</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.35">
-      <c r="B19" s="78" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B18" s="78" t="s">
         <v>286</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C18" s="85" t="s">
         <v>318</v>
       </c>
-      <c r="D19" s="103">
-        <f>(D12-D13)</f>
+      <c r="D18" s="103">
+        <f>(D5-D7-D12)</f>
         <v>-483600</v>
       </c>
-      <c r="E19" s="107">
-        <f>(E12-E13)</f>
+      <c r="E18" s="107">
+        <f t="shared" ref="E18:F18" si="1">(E5-E7-E12)</f>
         <v>124500</v>
       </c>
-      <c r="F19" s="107">
-        <f>(F12-F13)</f>
+      <c r="F18" s="107">
+        <f t="shared" si="1"/>
         <v>347200</v>
       </c>
     </row>

</xml_diff>